<commit_message>
part of ch6 solution
</commit_message>
<xml_diff>
--- a/docs/caffe2/cuda/Programming Massively Parallel Processors/images/coalesced_load.xlsx
+++ b/docs/caffe2/cuda/Programming Massively Parallel Processors/images/coalesced_load.xlsx
@@ -438,10 +438,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:Q74"/>
+  <dimension ref="A2:Q82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E67" activeCellId="0" sqref="67:67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D75" activeCellId="0" sqref="75:75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4059,6 +4059,462 @@
         <v>1</v>
       </c>
     </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <f aca="false">B75*2 + E75</f>
+        <v>2</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <f aca="false">A75 * 2 + D75</f>
+        <v>2</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <f aca="false">D75</f>
+        <v>0</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <f aca="false">E75</f>
+        <v>0</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <f aca="false">F75</f>
+        <v>2</v>
+      </c>
+      <c r="K75" s="0" t="n">
+        <f aca="false">C75 * 2 + D75</f>
+        <v>0</v>
+      </c>
+      <c r="L75" s="0" t="n">
+        <f aca="false">D75</f>
+        <v>0</v>
+      </c>
+      <c r="M75" s="0" t="n">
+        <f aca="false">E75</f>
+        <v>0</v>
+      </c>
+      <c r="N75" s="0" t="n">
+        <f aca="false">C75*2 + E75</f>
+        <v>0</v>
+      </c>
+      <c r="O75" s="0" t="n">
+        <f aca="false">G75</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <f aca="false">B76*2 + E76</f>
+        <v>2</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <f aca="false">A76 * 2 + D76</f>
+        <v>3</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <f aca="false">D76</f>
+        <v>1</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <f aca="false">E76</f>
+        <v>0</v>
+      </c>
+      <c r="J76" s="0" t="n">
+        <f aca="false">F76</f>
+        <v>2</v>
+      </c>
+      <c r="K76" s="0" t="n">
+        <f aca="false">C76 * 2 + D76</f>
+        <v>1</v>
+      </c>
+      <c r="L76" s="0" t="n">
+        <f aca="false">D76</f>
+        <v>1</v>
+      </c>
+      <c r="M76" s="0" t="n">
+        <f aca="false">E76</f>
+        <v>0</v>
+      </c>
+      <c r="N76" s="0" t="n">
+        <f aca="false">C76*2 + E76</f>
+        <v>0</v>
+      </c>
+      <c r="O76" s="0" t="n">
+        <f aca="false">G76</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <f aca="false">B77*2 + E77</f>
+        <v>3</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <f aca="false">A77 * 2 + D77</f>
+        <v>2</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <f aca="false">D77</f>
+        <v>0</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <f aca="false">E77</f>
+        <v>1</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <f aca="false">F77</f>
+        <v>3</v>
+      </c>
+      <c r="K77" s="0" t="n">
+        <f aca="false">C77 * 2 + D77</f>
+        <v>0</v>
+      </c>
+      <c r="L77" s="0" t="n">
+        <f aca="false">D77</f>
+        <v>0</v>
+      </c>
+      <c r="M77" s="0" t="n">
+        <f aca="false">E77</f>
+        <v>1</v>
+      </c>
+      <c r="N77" s="0" t="n">
+        <f aca="false">C77*2 + E77</f>
+        <v>1</v>
+      </c>
+      <c r="O77" s="0" t="n">
+        <f aca="false">G77</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <f aca="false">B78*2 + E78</f>
+        <v>3</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <f aca="false">A78 * 2 + D78</f>
+        <v>3</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <f aca="false">D78</f>
+        <v>1</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <f aca="false">E78</f>
+        <v>1</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <f aca="false">F78</f>
+        <v>3</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <f aca="false">C78 * 2 + D78</f>
+        <v>1</v>
+      </c>
+      <c r="L78" s="0" t="n">
+        <f aca="false">D78</f>
+        <v>1</v>
+      </c>
+      <c r="M78" s="0" t="n">
+        <f aca="false">E78</f>
+        <v>1</v>
+      </c>
+      <c r="N78" s="0" t="n">
+        <f aca="false">C78*2 + E78</f>
+        <v>1</v>
+      </c>
+      <c r="O78" s="0" t="n">
+        <f aca="false">G78</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <f aca="false">B79*2 + E79</f>
+        <v>2</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <f aca="false">A79 * 2 + D79</f>
+        <v>2</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <f aca="false">D79</f>
+        <v>0</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <f aca="false">E79</f>
+        <v>0</v>
+      </c>
+      <c r="J79" s="0" t="n">
+        <f aca="false">F79</f>
+        <v>2</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <f aca="false">C79 * 2 + D79</f>
+        <v>2</v>
+      </c>
+      <c r="L79" s="0" t="n">
+        <f aca="false">D79</f>
+        <v>0</v>
+      </c>
+      <c r="M79" s="0" t="n">
+        <f aca="false">E79</f>
+        <v>0</v>
+      </c>
+      <c r="N79" s="0" t="n">
+        <f aca="false">C79*2 + E79</f>
+        <v>2</v>
+      </c>
+      <c r="O79" s="0" t="n">
+        <f aca="false">G79</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <f aca="false">B80*2 + E80</f>
+        <v>2</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <f aca="false">A80 * 2 + D80</f>
+        <v>3</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <f aca="false">D80</f>
+        <v>1</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <f aca="false">E80</f>
+        <v>0</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <f aca="false">F80</f>
+        <v>2</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <f aca="false">C80 * 2 + D80</f>
+        <v>3</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <f aca="false">D80</f>
+        <v>1</v>
+      </c>
+      <c r="M80" s="0" t="n">
+        <f aca="false">E80</f>
+        <v>0</v>
+      </c>
+      <c r="N80" s="0" t="n">
+        <f aca="false">C80*2 + E80</f>
+        <v>2</v>
+      </c>
+      <c r="O80" s="0" t="n">
+        <f aca="false">G80</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <f aca="false">B81*2 + E81</f>
+        <v>3</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <f aca="false">A81 * 2 + D81</f>
+        <v>2</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <f aca="false">D81</f>
+        <v>0</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <f aca="false">E81</f>
+        <v>1</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <f aca="false">F81</f>
+        <v>3</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <f aca="false">C81 * 2 + D81</f>
+        <v>2</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <f aca="false">D81</f>
+        <v>0</v>
+      </c>
+      <c r="M81" s="0" t="n">
+        <f aca="false">E81</f>
+        <v>1</v>
+      </c>
+      <c r="N81" s="0" t="n">
+        <f aca="false">C81*2 + E81</f>
+        <v>3</v>
+      </c>
+      <c r="O81" s="0" t="n">
+        <f aca="false">G81</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <f aca="false">B82*2 + E82</f>
+        <v>3</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <f aca="false">A82 * 2 + D82</f>
+        <v>3</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <f aca="false">D82</f>
+        <v>1</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <f aca="false">E82</f>
+        <v>1</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <f aca="false">F82</f>
+        <v>3</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <f aca="false">C82 * 2 + D82</f>
+        <v>3</v>
+      </c>
+      <c r="L82" s="0" t="n">
+        <f aca="false">D82</f>
+        <v>1</v>
+      </c>
+      <c r="M82" s="0" t="n">
+        <f aca="false">E82</f>
+        <v>1</v>
+      </c>
+      <c r="N82" s="0" t="n">
+        <f aca="false">C82*2 + E82</f>
+        <v>3</v>
+      </c>
+      <c r="O82" s="0" t="n">
+        <f aca="false">G82</f>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:B5"/>

</xml_diff>